<commit_message>
Actualizacion clse 3 y agregar clase 3 en R
</commit_message>
<xml_diff>
--- a/Data Pre processing/mpg_clean.xlsx
+++ b/Data Pre processing/mpg_clean.xlsx
@@ -679,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I399"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,1120 +1484,6 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-    </row>
-    <row r="69" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-    </row>
-    <row r="80" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-    </row>
-    <row r="81" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-    </row>
-    <row r="82" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-    </row>
-    <row r="94" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="95" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-    </row>
-    <row r="97" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-    </row>
-    <row r="99" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-    </row>
-    <row r="100" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="103" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-    </row>
-    <row r="104" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-    </row>
-    <row r="105" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-    </row>
-    <row r="106" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-    </row>
-    <row r="107" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-    </row>
-    <row r="108" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-    </row>
-    <row r="109" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-    </row>
-    <row r="110" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-    </row>
-    <row r="111" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-    </row>
-    <row r="112" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-    </row>
-    <row r="113" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-    </row>
-    <row r="117" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-    </row>
-    <row r="119" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
-    </row>
-    <row r="121" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
-    </row>
-    <row r="123" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-    </row>
-    <row r="127" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
-    </row>
-    <row r="128" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
-    </row>
-    <row r="133" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="139" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="140" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
-    </row>
-    <row r="141" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
-    </row>
-    <row r="142" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
-    </row>
-    <row r="149" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
-    </row>
-    <row r="150" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
-    </row>
-    <row r="154" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
-    </row>
-    <row r="158" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
-    </row>
-    <row r="160" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
-    </row>
-    <row r="162" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A163" s="1"/>
-    </row>
-    <row r="164" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A164" s="1"/>
-    </row>
-    <row r="165" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
-    </row>
-    <row r="166" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
-    </row>
-    <row r="167" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
-    </row>
-    <row r="168" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
-    </row>
-    <row r="169" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A169" s="1"/>
-    </row>
-    <row r="170" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
-    </row>
-    <row r="171" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A171" s="1"/>
-    </row>
-    <row r="172" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A173" s="1"/>
-    </row>
-    <row r="174" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="175" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A175" s="1"/>
-    </row>
-    <row r="176" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A176" s="1"/>
-    </row>
-    <row r="177" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="178" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A184" s="1"/>
-    </row>
-    <row r="185" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A185" s="1"/>
-    </row>
-    <row r="186" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A193" s="1"/>
-    </row>
-    <row r="194" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A194" s="1"/>
-    </row>
-    <row r="195" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A197" s="1"/>
-    </row>
-    <row r="198" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A198" s="1"/>
-    </row>
-    <row r="199" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A200" s="1"/>
-    </row>
-    <row r="201" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A201" s="1"/>
-    </row>
-    <row r="202" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A202" s="1"/>
-    </row>
-    <row r="203" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A203" s="1"/>
-    </row>
-    <row r="204" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A204" s="1"/>
-    </row>
-    <row r="205" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A205" s="1"/>
-    </row>
-    <row r="206" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A206" s="1"/>
-    </row>
-    <row r="207" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A207" s="1"/>
-    </row>
-    <row r="208" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A208" s="1"/>
-    </row>
-    <row r="209" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A209" s="1"/>
-    </row>
-    <row r="210" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A210" s="1"/>
-    </row>
-    <row r="211" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A211" s="1"/>
-    </row>
-    <row r="212" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A212" s="1"/>
-    </row>
-    <row r="213" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A213" s="1"/>
-    </row>
-    <row r="214" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A214" s="1"/>
-    </row>
-    <row r="215" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A215" s="1"/>
-    </row>
-    <row r="216" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A216" s="1"/>
-    </row>
-    <row r="217" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A217" s="1"/>
-    </row>
-    <row r="218" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A218" s="1"/>
-    </row>
-    <row r="219" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A219" s="1"/>
-    </row>
-    <row r="220" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A220" s="1"/>
-    </row>
-    <row r="221" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A221" s="1"/>
-    </row>
-    <row r="222" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A222" s="1"/>
-    </row>
-    <row r="223" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A223" s="1"/>
-    </row>
-    <row r="224" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A224" s="1"/>
-    </row>
-    <row r="225" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A225" s="1"/>
-    </row>
-    <row r="226" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A226" s="1"/>
-    </row>
-    <row r="227" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A227" s="1"/>
-    </row>
-    <row r="228" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A228" s="1"/>
-    </row>
-    <row r="229" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A229" s="1"/>
-    </row>
-    <row r="230" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A230" s="1"/>
-    </row>
-    <row r="231" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A231" s="1"/>
-    </row>
-    <row r="232" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A232" s="1"/>
-    </row>
-    <row r="233" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A233" s="1"/>
-    </row>
-    <row r="234" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A234" s="1"/>
-    </row>
-    <row r="235" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A235" s="1"/>
-    </row>
-    <row r="236" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A236" s="1"/>
-    </row>
-    <row r="237" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A237" s="1"/>
-    </row>
-    <row r="238" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A238" s="1"/>
-    </row>
-    <row r="239" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A239" s="1"/>
-    </row>
-    <row r="240" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A240" s="1"/>
-    </row>
-    <row r="241" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A241" s="1"/>
-    </row>
-    <row r="242" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A242" s="1"/>
-    </row>
-    <row r="243" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A243" s="1"/>
-    </row>
-    <row r="244" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A244" s="1"/>
-    </row>
-    <row r="245" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A245" s="1"/>
-    </row>
-    <row r="246" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A246" s="1"/>
-    </row>
-    <row r="247" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A247" s="1"/>
-    </row>
-    <row r="248" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A248" s="1"/>
-    </row>
-    <row r="249" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A249" s="1"/>
-    </row>
-    <row r="250" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A250" s="1"/>
-    </row>
-    <row r="251" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A251" s="1"/>
-    </row>
-    <row r="252" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A252" s="1"/>
-    </row>
-    <row r="253" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A253" s="1"/>
-    </row>
-    <row r="254" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A254" s="1"/>
-    </row>
-    <row r="255" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A255" s="1"/>
-    </row>
-    <row r="256" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A256" s="1"/>
-    </row>
-    <row r="257" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A257" s="1"/>
-    </row>
-    <row r="258" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A258" s="1"/>
-    </row>
-    <row r="259" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A259" s="1"/>
-    </row>
-    <row r="260" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A260" s="1"/>
-    </row>
-    <row r="261" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A261" s="1"/>
-    </row>
-    <row r="262" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A262" s="1"/>
-    </row>
-    <row r="263" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A263" s="1"/>
-    </row>
-    <row r="264" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A264" s="1"/>
-    </row>
-    <row r="265" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A265" s="1"/>
-    </row>
-    <row r="266" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A266" s="1"/>
-    </row>
-    <row r="267" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A267" s="1"/>
-    </row>
-    <row r="268" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A268" s="1"/>
-    </row>
-    <row r="269" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A269" s="1"/>
-    </row>
-    <row r="270" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A270" s="1"/>
-    </row>
-    <row r="271" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A271" s="1"/>
-    </row>
-    <row r="272" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A272" s="1"/>
-    </row>
-    <row r="273" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A273" s="1"/>
-    </row>
-    <row r="274" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A274" s="1"/>
-    </row>
-    <row r="275" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A275" s="1"/>
-    </row>
-    <row r="276" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A276" s="1"/>
-    </row>
-    <row r="277" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A277" s="1"/>
-    </row>
-    <row r="278" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A278" s="1"/>
-    </row>
-    <row r="279" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A279" s="1"/>
-    </row>
-    <row r="280" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A280" s="1"/>
-    </row>
-    <row r="281" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A281" s="1"/>
-    </row>
-    <row r="282" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A282" s="1"/>
-    </row>
-    <row r="283" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A283" s="1"/>
-    </row>
-    <row r="284" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A284" s="1"/>
-    </row>
-    <row r="285" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A285" s="1"/>
-    </row>
-    <row r="286" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A286" s="1"/>
-    </row>
-    <row r="287" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A287" s="1"/>
-    </row>
-    <row r="288" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A288" s="1"/>
-    </row>
-    <row r="289" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A289" s="1"/>
-    </row>
-    <row r="290" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A290" s="1"/>
-    </row>
-    <row r="291" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A291" s="1"/>
-    </row>
-    <row r="292" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A292" s="1"/>
-    </row>
-    <row r="293" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A293" s="1"/>
-    </row>
-    <row r="294" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A294" s="1"/>
-    </row>
-    <row r="295" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A295" s="1"/>
-    </row>
-    <row r="296" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A296" s="1"/>
-    </row>
-    <row r="297" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A297" s="1"/>
-    </row>
-    <row r="298" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A298" s="1"/>
-    </row>
-    <row r="299" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A299" s="1"/>
-    </row>
-    <row r="300" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A300" s="1"/>
-    </row>
-    <row r="301" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A301" s="1"/>
-    </row>
-    <row r="302" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A302" s="1"/>
-    </row>
-    <row r="303" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A303" s="1"/>
-    </row>
-    <row r="304" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A304" s="1"/>
-    </row>
-    <row r="305" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A305" s="1"/>
-    </row>
-    <row r="306" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A306" s="1"/>
-    </row>
-    <row r="307" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A307" s="1"/>
-    </row>
-    <row r="308" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A308" s="1"/>
-    </row>
-    <row r="309" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A309" s="1"/>
-    </row>
-    <row r="310" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A310" s="1"/>
-    </row>
-    <row r="311" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A311" s="1"/>
-    </row>
-    <row r="312" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A312" s="1"/>
-    </row>
-    <row r="313" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A313" s="1"/>
-    </row>
-    <row r="314" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A314" s="1"/>
-    </row>
-    <row r="315" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A315" s="1"/>
-    </row>
-    <row r="316" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A316" s="1"/>
-    </row>
-    <row r="317" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A317" s="1"/>
-    </row>
-    <row r="318" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A318" s="1"/>
-    </row>
-    <row r="319" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A319" s="1"/>
-    </row>
-    <row r="320" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A320" s="1"/>
-    </row>
-    <row r="321" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A321" s="1"/>
-    </row>
-    <row r="322" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A322" s="1"/>
-    </row>
-    <row r="323" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A323" s="1"/>
-    </row>
-    <row r="324" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A324" s="1"/>
-    </row>
-    <row r="325" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A325" s="1"/>
-    </row>
-    <row r="326" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A326" s="1"/>
-    </row>
-    <row r="327" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A327" s="1"/>
-    </row>
-    <row r="328" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A328" s="1"/>
-    </row>
-    <row r="329" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A329" s="1"/>
-    </row>
-    <row r="330" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A330" s="1"/>
-    </row>
-    <row r="331" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A331" s="1"/>
-    </row>
-    <row r="332" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A332" s="1"/>
-    </row>
-    <row r="333" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A333" s="1"/>
-    </row>
-    <row r="334" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A334" s="1"/>
-    </row>
-    <row r="335" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A335" s="1"/>
-    </row>
-    <row r="336" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A336" s="1"/>
-    </row>
-    <row r="337" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A337" s="1"/>
-    </row>
-    <row r="338" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A338" s="1"/>
-    </row>
-    <row r="339" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A339" s="1"/>
-    </row>
-    <row r="340" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A340" s="1"/>
-    </row>
-    <row r="341" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A341" s="1"/>
-    </row>
-    <row r="342" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A342" s="1"/>
-    </row>
-    <row r="343" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A343" s="1"/>
-    </row>
-    <row r="344" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A344" s="1"/>
-    </row>
-    <row r="345" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A345" s="1"/>
-    </row>
-    <row r="346" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A346" s="1"/>
-    </row>
-    <row r="347" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A347" s="1"/>
-    </row>
-    <row r="348" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A348" s="1"/>
-    </row>
-    <row r="349" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A349" s="1"/>
-    </row>
-    <row r="350" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A350" s="1"/>
-    </row>
-    <row r="351" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A351" s="1"/>
-    </row>
-    <row r="352" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A352" s="1"/>
-    </row>
-    <row r="353" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A353" s="1"/>
-    </row>
-    <row r="354" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A354" s="1"/>
-    </row>
-    <row r="355" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A355" s="1"/>
-    </row>
-    <row r="356" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A356" s="1"/>
-    </row>
-    <row r="357" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A357" s="1"/>
-    </row>
-    <row r="358" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A358" s="1"/>
-    </row>
-    <row r="359" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A359" s="1"/>
-    </row>
-    <row r="360" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A360" s="1"/>
-    </row>
-    <row r="361" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A361" s="1"/>
-    </row>
-    <row r="362" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A362" s="1"/>
-    </row>
-    <row r="363" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A363" s="1"/>
-    </row>
-    <row r="364" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A364" s="1"/>
-    </row>
-    <row r="365" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A365" s="1"/>
-    </row>
-    <row r="366" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A366" s="1"/>
-    </row>
-    <row r="367" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A367" s="1"/>
-    </row>
-    <row r="368" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A368" s="1"/>
-    </row>
-    <row r="369" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A369" s="1"/>
-    </row>
-    <row r="370" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A370" s="1"/>
-    </row>
-    <row r="371" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A371" s="1"/>
-    </row>
-    <row r="372" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A372" s="1"/>
-    </row>
-    <row r="373" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A373" s="1"/>
-    </row>
-    <row r="374" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A374" s="1"/>
-    </row>
-    <row r="375" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A375" s="1"/>
-    </row>
-    <row r="376" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A376" s="1"/>
-    </row>
-    <row r="377" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A377" s="1"/>
-    </row>
-    <row r="378" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A378" s="1"/>
-    </row>
-    <row r="379" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A379" s="1"/>
-    </row>
-    <row r="380" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A380" s="1"/>
-    </row>
-    <row r="381" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A381" s="1"/>
-    </row>
-    <row r="382" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A382" s="1"/>
-    </row>
-    <row r="383" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A383" s="1"/>
-    </row>
-    <row r="384" spans="1:1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A384" s="1"/>
-    </row>
-    <row r="385" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A385" s="1"/>
-    </row>
-    <row r="386" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A386" s="1"/>
-    </row>
-    <row r="387" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A387" s="1"/>
-    </row>
-    <row r="388" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A388" s="1"/>
-    </row>
-    <row r="389" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A389" s="1"/>
-    </row>
-    <row r="390" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A390" s="1"/>
-    </row>
-    <row r="391" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A391" s="1"/>
-      <c r="F391" s="2"/>
-    </row>
-    <row r="392" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A392" s="1"/>
-    </row>
-    <row r="393" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A393" s="1"/>
-    </row>
-    <row r="394" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A394" s="1"/>
-    </row>
-    <row r="395" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A395" s="1"/>
-    </row>
-    <row r="396" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A396" s="1"/>
-    </row>
-    <row r="397" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A397" s="1"/>
-    </row>
-    <row r="398" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A398" s="1"/>
-    </row>
-    <row r="399" spans="1:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="A399" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>